<commit_message>
Remove graph dependency on actual data values. Finish non-perturbable test for graph.
</commit_message>
<xml_diff>
--- a/NoSheetTests/TestData/RangeVariations.xlsx
+++ b/NoSheetTests/TestData/RangeVariations.xlsx
@@ -350,7 +350,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -389,6 +389,10 @@
         <f>A3</f>
         <v>3</v>
       </c>
+      <c r="C3">
+        <f>SUM(A1:A4)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">

</xml_diff>